<commit_message>
small changes to curated data file
</commit_message>
<xml_diff>
--- a/curatedafg_100.xlsx
+++ b/curatedafg_100.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cody/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crn2k\Documents\lda-lsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17595" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="curatedafg_100" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="129">
   <si>
     <t>Enemy Action</t>
   </si>
@@ -265,9 +262,6 @@
   </si>
   <si>
     <t>EXPLOSION IN SAKIHAN KALAY</t>
-  </si>
-  <si>
-    <t>Turn In</t>
   </si>
   <si>
     <t>(S//REL GCTF) IED IVO KANDAHAR PRT SITE: ON 11 JAN 03, WORKERS AT THE KANDAHAR CITY PRT SITE IVO N3137.539 E06544.338 DISCOVERED AN IED.  THE ACM BURIED THE IED BETWEEN 500M-750M FROM THE PRT SITE ON THE SIDE OF A DIRT ROAD FREQUENTLY USED BY THE PRT WORKERS.  THE IED CONSISTED OF 122MM ARTILLERY ROUND WITH AN ELECTRICALLY CHARGED WIRELESS DOORBELL RINGER DETONATION SWITCH.  THE STANDOFF CAPABILITY OF THIS DEVICE IS APPROXIMATELY 100 METERS BASED OFF THE ELECTRICAL WIRING, BATTERIES, AND DOORBELL SPEAKER LOCATIONS.</t>
@@ -479,6 +473,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -749,11 +746,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.5" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -763,11 +768,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -777,11 +782,11 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="283.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -795,7 +800,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -805,11 +810,11 @@
       <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -819,11 +824,11 @@
       <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -833,11 +838,11 @@
       <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -847,11 +852,11 @@
       <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -861,11 +866,11 @@
       <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -875,11 +880,11 @@
       <c r="C9" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -889,11 +894,11 @@
       <c r="C10" t="s">
         <v>6</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -903,11 +908,11 @@
       <c r="C11" t="s">
         <v>6</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -917,11 +922,11 @@
       <c r="C12" t="s">
         <v>6</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -931,11 +936,11 @@
       <c r="C13" t="s">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -945,11 +950,11 @@
       <c r="C14" t="s">
         <v>30</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="362.25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -963,7 +968,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -973,11 +978,11 @@
       <c r="C16" t="s">
         <v>34</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -987,11 +992,11 @@
       <c r="C17" t="s">
         <v>30</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1001,11 +1006,11 @@
       <c r="C18" t="s">
         <v>38</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -1015,11 +1020,11 @@
       <c r="C19" t="s">
         <v>41</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1029,11 +1034,11 @@
       <c r="C20" t="s">
         <v>30</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1043,11 +1048,11 @@
       <c r="C21" t="s">
         <v>30</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1057,11 +1062,11 @@
       <c r="C22" t="s">
         <v>41</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1071,11 +1076,11 @@
       <c r="C23" t="s">
         <v>41</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1085,11 +1090,11 @@
       <c r="C24" t="s">
         <v>41</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1103,7 +1108,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1113,11 +1118,11 @@
       <c r="C26" t="s">
         <v>2</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1127,11 +1132,11 @@
       <c r="C27" t="s">
         <v>20</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1141,11 +1146,11 @@
       <c r="C28" t="s">
         <v>20</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1155,11 +1160,11 @@
       <c r="C29" t="s">
         <v>51</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1169,11 +1174,11 @@
       <c r="C30" t="s">
         <v>41</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1183,11 +1188,11 @@
       <c r="C31" t="s">
         <v>6</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1197,11 +1202,11 @@
       <c r="C32" t="s">
         <v>6</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -1211,11 +1216,11 @@
       <c r="C33" t="s">
         <v>57</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -1225,11 +1230,11 @@
       <c r="C34" t="s">
         <v>10</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -1239,11 +1244,11 @@
       <c r="C35" t="s">
         <v>6</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -1253,11 +1258,11 @@
       <c r="C36" t="s">
         <v>61</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -1271,7 +1276,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -1281,11 +1286,11 @@
       <c r="C38" t="s">
         <v>6</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -1295,11 +1300,11 @@
       <c r="C39" t="s">
         <v>6</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -1309,11 +1314,11 @@
       <c r="C40" t="s">
         <v>20</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -1323,11 +1328,11 @@
       <c r="C41" t="s">
         <v>2</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -1337,11 +1342,11 @@
       <c r="C42" t="s">
         <v>6</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -1351,11 +1356,11 @@
       <c r="C43" t="s">
         <v>6</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -1365,11 +1370,11 @@
       <c r="C44" t="s">
         <v>6</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -1379,11 +1384,11 @@
       <c r="C45" t="s">
         <v>20</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -1393,11 +1398,11 @@
       <c r="C46" t="s">
         <v>20</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -1407,11 +1412,11 @@
       <c r="C47" t="s">
         <v>6</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -1421,11 +1426,11 @@
       <c r="C48" t="s">
         <v>6</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -1435,11 +1440,11 @@
       <c r="C49" t="s">
         <v>6</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>28</v>
       </c>
@@ -1449,53 +1454,53 @@
       <c r="C50" t="s">
         <v>57</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>28</v>
       </c>
       <c r="B51" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="C51" t="s">
         <v>41</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>4</v>
-      </c>
-      <c r="B52" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" t="s">
+    <row r="53" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>4</v>
-      </c>
-      <c r="B53" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>0</v>
       </c>
@@ -1505,11 +1510,11 @@
       <c r="C54" t="s">
         <v>2</v>
       </c>
-      <c r="D54" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D54" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="126" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -1519,109 +1524,109 @@
       <c r="C55" t="s">
         <v>16</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>4</v>
-      </c>
-      <c r="B56" t="s">
-        <v>5</v>
-      </c>
-      <c r="C56" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="B57" t="s">
         <v>84</v>
-      </c>
-      <c r="B57" t="s">
-        <v>85</v>
       </c>
       <c r="C57" t="s">
         <v>22</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="267.75" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>4</v>
-      </c>
-      <c r="B58" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" t="s">
+    <row r="59" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>4</v>
-      </c>
-      <c r="B59" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" t="s">
+    <row r="60" spans="1:4" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>4</v>
-      </c>
-      <c r="B60" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" t="s">
+    <row r="61" spans="1:4" ht="299.25" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>4</v>
-      </c>
-      <c r="B61" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" t="s">
-        <v>6</v>
-      </c>
-      <c r="D61" s="1" t="s">
+    <row r="62" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>4</v>
-      </c>
-      <c r="B62" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" t="s">
-        <v>6</v>
-      </c>
-      <c r="D62" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>0</v>
       </c>
@@ -1631,11 +1636,11 @@
       <c r="C63" t="s">
         <v>2</v>
       </c>
-      <c r="D63" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D63" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="126" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>0</v>
       </c>
@@ -1645,11 +1650,11 @@
       <c r="C64" t="s">
         <v>20</v>
       </c>
-      <c r="D64" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D64" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>0</v>
       </c>
@@ -1659,11 +1664,11 @@
       <c r="C65" t="s">
         <v>2</v>
       </c>
-      <c r="D65" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D65" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>0</v>
       </c>
@@ -1673,25 +1678,25 @@
       <c r="C66" t="s">
         <v>2</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>4</v>
+      </c>
+      <c r="B67" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>4</v>
-      </c>
-      <c r="B67" t="s">
-        <v>5</v>
-      </c>
-      <c r="C67" t="s">
-        <v>6</v>
-      </c>
-      <c r="D67" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>0</v>
       </c>
@@ -1701,25 +1706,25 @@
       <c r="C68" t="s">
         <v>2</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>4</v>
-      </c>
-      <c r="B69" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" t="s">
-        <v>6</v>
-      </c>
-      <c r="D69" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>0</v>
       </c>
@@ -1729,67 +1734,67 @@
       <c r="C70" t="s">
         <v>20</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>4</v>
+      </c>
+      <c r="B71" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>4</v>
-      </c>
-      <c r="B71" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" t="s">
-        <v>6</v>
-      </c>
-      <c r="D71" t="s">
+    <row r="72" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>4</v>
-      </c>
-      <c r="B72" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" t="s">
-        <v>6</v>
-      </c>
-      <c r="D72" t="s">
+    <row r="73" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>4</v>
+      </c>
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>4</v>
-      </c>
-      <c r="B73" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" t="s">
-        <v>6</v>
-      </c>
-      <c r="D73" t="s">
+    <row r="74" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>4</v>
-      </c>
-      <c r="B74" t="s">
-        <v>5</v>
-      </c>
-      <c r="C74" t="s">
-        <v>6</v>
-      </c>
-      <c r="D74" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>0</v>
       </c>
@@ -1799,25 +1804,25 @@
       <c r="C75" t="s">
         <v>2</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="189" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>4</v>
+      </c>
+      <c r="B76" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>4</v>
-      </c>
-      <c r="B76" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D76" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>0</v>
       </c>
@@ -1827,11 +1832,11 @@
       <c r="C77" t="s">
         <v>2</v>
       </c>
-      <c r="D77" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D77" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>0</v>
       </c>
@@ -1839,27 +1844,27 @@
         <v>1</v>
       </c>
       <c r="C78" t="s">
+        <v>106</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D78" t="s">
+    </row>
+    <row r="79" spans="1:4" ht="189" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>4</v>
+      </c>
+      <c r="B79" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>4</v>
-      </c>
-      <c r="B79" t="s">
-        <v>5</v>
-      </c>
-      <c r="C79" t="s">
-        <v>6</v>
-      </c>
-      <c r="D79" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" ht="126" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>14</v>
       </c>
@@ -1869,25 +1874,25 @@
       <c r="C80" t="s">
         <v>16</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="204.75" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>4</v>
+      </c>
+      <c r="B81" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>4</v>
-      </c>
-      <c r="B81" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" t="s">
-        <v>6</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>0</v>
       </c>
@@ -1898,10 +1903,10 @@
         <v>20</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>0</v>
       </c>
@@ -1911,25 +1916,25 @@
       <c r="C83" t="s">
         <v>2</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D83" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>4</v>
+      </c>
+      <c r="B84" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" t="s">
+        <v>6</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>4</v>
-      </c>
-      <c r="B84" t="s">
-        <v>5</v>
-      </c>
-      <c r="C84" t="s">
-        <v>6</v>
-      </c>
-      <c r="D84" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>0</v>
       </c>
@@ -1939,25 +1944,25 @@
       <c r="C85" t="s">
         <v>2</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>4</v>
+      </c>
+      <c r="B86" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>4</v>
-      </c>
-      <c r="B86" t="s">
-        <v>5</v>
-      </c>
-      <c r="C86" t="s">
-        <v>6</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>0</v>
       </c>
@@ -1967,95 +1972,95 @@
       <c r="C87" t="s">
         <v>2</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" t="s">
+        <v>6</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>4</v>
-      </c>
-      <c r="B88" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" t="s">
-        <v>6</v>
-      </c>
-      <c r="D88" t="s">
+    <row r="89" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>4</v>
+      </c>
+      <c r="B89" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>4</v>
-      </c>
-      <c r="B89" t="s">
-        <v>5</v>
-      </c>
-      <c r="C89" t="s">
-        <v>6</v>
-      </c>
-      <c r="D89" t="s">
+    <row r="90" spans="1:4" ht="315" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>4</v>
+      </c>
+      <c r="B90" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" t="s">
+        <v>6</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>4</v>
-      </c>
-      <c r="B90" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" t="s">
-        <v>6</v>
-      </c>
-      <c r="D90" s="1" t="s">
+    <row r="91" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>4</v>
+      </c>
+      <c r="B91" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>4</v>
-      </c>
-      <c r="B91" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91" t="s">
-        <v>6</v>
-      </c>
-      <c r="D91" t="s">
+    <row r="92" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>4</v>
+      </c>
+      <c r="B92" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>4</v>
-      </c>
-      <c r="B92" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" t="s">
-        <v>6</v>
-      </c>
-      <c r="D92" t="s">
+    <row r="93" spans="1:4" ht="189" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>4</v>
+      </c>
+      <c r="B93" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" t="s">
+        <v>6</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>4</v>
-      </c>
-      <c r="B93" t="s">
-        <v>5</v>
-      </c>
-      <c r="C93" t="s">
-        <v>6</v>
-      </c>
-      <c r="D93" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>0</v>
       </c>
@@ -2065,11 +2070,11 @@
       <c r="C94" t="s">
         <v>2</v>
       </c>
-      <c r="D94" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D94" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>0</v>
       </c>
@@ -2079,11 +2084,11 @@
       <c r="C95" t="s">
         <v>2</v>
       </c>
-      <c r="D95" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D95" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>4</v>
       </c>
@@ -2093,11 +2098,11 @@
       <c r="C96" t="s">
         <v>22</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>4</v>
       </c>
@@ -2107,25 +2112,25 @@
       <c r="C97" t="s">
         <v>6</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>4</v>
+      </c>
+      <c r="B98" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" t="s">
+        <v>6</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
-        <v>4</v>
-      </c>
-      <c r="B98" t="s">
-        <v>5</v>
-      </c>
-      <c r="C98" t="s">
-        <v>6</v>
-      </c>
-      <c r="D98" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>0</v>
       </c>
@@ -2135,11 +2140,11 @@
       <c r="C99" t="s">
         <v>20</v>
       </c>
-      <c r="D99" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D99" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>8</v>
       </c>
@@ -2149,8 +2154,8 @@
       <c r="C100" t="s">
         <v>10</v>
       </c>
-      <c r="D100" t="s">
-        <v>129</v>
+      <c r="D100" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>